<commit_message>
Finalização FPA - Pontos ajustados
</commit_message>
<xml_diff>
--- a/3SIT-FerramentaFPA-ProfRJP-Automatica-Lock.xlsx
+++ b/3SIT-FerramentaFPA-ProfRJP-Automatica-Lock.xlsx
@@ -5,20 +5,21 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\labsfiap\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\labsfiap\Downloads\Aula-FTP-Classificacao-Funcional-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820C3E11-8733-4310-B6CE-78949D688A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C4C1D0-B1C4-42D7-8EFC-EFBDBECECDFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pontos Nao Ajustados" sheetId="1" r:id="rId1"/>
     <sheet name="Pontos Ajustados" sheetId="6" r:id="rId2"/>
-    <sheet name="Lista DER" sheetId="3" state="hidden" r:id="rId3"/>
-    <sheet name="Complexidade" sheetId="4" r:id="rId4"/>
-    <sheet name="Pontuação" sheetId="5" r:id="rId5"/>
-    <sheet name="Seletores" sheetId="2" state="hidden" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId3"/>
+    <sheet name="Lista DER" sheetId="3" state="hidden" r:id="rId4"/>
+    <sheet name="Complexidade" sheetId="4" r:id="rId5"/>
+    <sheet name="Pontuação" sheetId="5" r:id="rId6"/>
+    <sheet name="Seletores" sheetId="2" state="hidden" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="97">
   <si>
     <t>COMPONENTE FUNCIONAL BÁSICO (CFB)</t>
   </si>
@@ -331,6 +332,15 @@
   </si>
   <si>
     <t>Descrição do Problema</t>
+  </si>
+  <si>
+    <t>Facilidade de treinamento</t>
+  </si>
+  <si>
+    <t>"Uso de APIs"</t>
+  </si>
+  <si>
+    <t>máquinas robustas</t>
   </si>
 </sst>
 </file>
@@ -1713,7 +1723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N424"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A234" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A228" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A250" sqref="A250"/>
     </sheetView>
   </sheetViews>
@@ -11163,8 +11173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11203,20 +11213,24 @@
       </c>
       <c r="F5">
         <f>0.65+(0.01*C20)</f>
-        <v>0.65</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="22">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="23"/>
+      <c r="C7" s="23">
+        <v>1</v>
+      </c>
       <c r="E7" t="s">
         <v>48</v>
       </c>
@@ -11229,80 +11243,104 @@
       <c r="B8" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="23"/>
+      <c r="C8" s="23">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="23"/>
+      <c r="C9" s="23">
+        <v>1</v>
+      </c>
       <c r="E9" s="12" t="s">
         <v>47</v>
       </c>
       <c r="F9" s="12">
         <f>F5*F7</f>
-        <v>35.1</v>
+        <v>50.220000000000006</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="23"/>
+      <c r="C10" s="23">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="23"/>
+      <c r="C11" s="23">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="23"/>
+      <c r="C12" s="23">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="23"/>
+      <c r="C13" s="23">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="23"/>
+      <c r="C14" s="23">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="23"/>
+      <c r="C15" s="23">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="23"/>
+      <c r="C16" s="23">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="23"/>
+      <c r="C17" s="23">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="23"/>
+      <c r="C18" s="23">
+        <v>3</v>
+      </c>
     </row>
     <row r="19" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="24"/>
+      <c r="C19" s="24">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="2:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="13" t="s">
@@ -11310,7 +11348,7 @@
       </c>
       <c r="C20" s="14">
         <f>SUM(C6:C19)</f>
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -11332,6 +11370,105 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{133F2C6B-E4C3-4BF8-8EF8-AF83BD4805AF}">
+  <dimension ref="C1:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B765"/>
   <sheetViews>
@@ -14413,7 +14550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -14445,7 +14582,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -14477,7 +14614,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K201"/>
   <sheetViews>

</xml_diff>